<commit_message>
trabalhando ainda no metodo de carregar arquivo CSV
</commit_message>
<xml_diff>
--- a/recursos/funcionarios.xlsx
+++ b/recursos/funcionarios.xlsx
@@ -92,10 +92,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="12" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -634,16 +632,16 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>43</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>1234</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>1294</v>
       </c>
     </row>
@@ -651,16 +649,16 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>56</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>4321</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>5259</v>
       </c>
     </row>
@@ -668,16 +666,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>23</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>2345</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>8576</v>
       </c>
     </row>
@@ -685,16 +683,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>42</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>5432</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>1300</v>
       </c>
     </row>
@@ -702,16 +700,16 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>33</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>3456</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>2349</v>
       </c>
     </row>
@@ -719,16 +717,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>61</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>6543</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>15256</v>
       </c>
     </row>
@@ -736,16 +734,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>28</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>4567</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>3419</v>
       </c>
     </row>
@@ -753,16 +751,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>31</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>7654</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>5107</v>
       </c>
     </row>
@@ -770,16 +768,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>24</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>5678</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>4007</v>
       </c>
     </row>
@@ -787,23 +785,23 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>37</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>8765</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>2900</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>